<commit_message>
scenario 03a + unit weapon sprites for brawler
</commit_message>
<xml_diff>
--- a/units/Durok/Damage.xlsx
+++ b/units/Durok/Damage.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c009ef319659ad0f/Dokumente/My Games/Wesnoth1.16/data/add-ons/deception/units/Durok/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="229" documentId="11_F25DC773A252ABDACC1048AA191E4DF65BDE58F1" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9E2F3BB4-6C62-4B22-84B1-C144EE5A8FF1}"/>
+  <xr:revisionPtr revIDLastSave="276" documentId="11_F25DC773A252ABDACC1048AA191E4DF65BDE58F1" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EB0F3911-83E6-4D07-AFFB-11249B0C3AF6}"/>
   <bookViews>
-    <workbookView xWindow="9520" yWindow="0" windowWidth="9760" windowHeight="12080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1180" windowWidth="19200" windowHeight="8433" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Type</t>
   </si>
@@ -73,6 +73,12 @@
   <si>
     <t>light_bolt</t>
   </si>
+  <si>
+    <t>elvish_spear2</t>
+  </si>
+  <si>
+    <t>elvish_sword</t>
+  </si>
 </sst>
 </file>
 
@@ -89,7 +95,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="9" tint="-0.499984740745262"/>
+      <color rgb="FF0070C0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -141,22 +147,22 @@
   </cellStyleXfs>
   <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -178,6 +184,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -443,853 +453,1007 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AF8"/>
+  <dimension ref="A1:AL8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="Q8" sqref="Q8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="W5" sqref="W5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="1" max="2" width="6.5859375" customWidth="1"/>
-    <col min="3" max="5" width="4.52734375" style="2" customWidth="1"/>
-    <col min="6" max="8" width="4.52734375" style="4" customWidth="1"/>
-    <col min="9" max="11" width="4.52734375" style="6" customWidth="1"/>
-    <col min="12" max="14" width="4.52734375" style="8" customWidth="1"/>
-    <col min="15" max="17" width="4.52734375" style="2" customWidth="1"/>
-    <col min="18" max="20" width="4.52734375" style="4" customWidth="1"/>
-    <col min="21" max="23" width="4.52734375" style="6" customWidth="1"/>
-    <col min="24" max="26" width="4.52734375" style="8" customWidth="1"/>
-    <col min="27" max="29" width="4.52734375" style="2" customWidth="1"/>
+    <col min="3" max="5" width="4.52734375" style="1" customWidth="1"/>
+    <col min="6" max="8" width="4.52734375" style="2" customWidth="1"/>
+    <col min="9" max="11" width="4.52734375" style="3" customWidth="1"/>
+    <col min="12" max="14" width="4.52734375" style="4" customWidth="1"/>
+    <col min="15" max="17" width="4.52734375" style="1" customWidth="1"/>
+    <col min="18" max="20" width="4.52734375" style="2" customWidth="1"/>
+    <col min="21" max="23" width="4.52734375" style="1" customWidth="1"/>
+    <col min="24" max="26" width="4.52734375" style="2" customWidth="1"/>
+    <col min="27" max="29" width="4.52734375" style="3" customWidth="1"/>
     <col min="30" max="32" width="4.52734375" style="4" customWidth="1"/>
+    <col min="33" max="35" width="4.52734375" style="1" customWidth="1"/>
+    <col min="36" max="38" width="4.52734375" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:38" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="7" t="s">
+      <c r="C1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="M1" s="7"/>
-      <c r="N1" s="7"/>
-      <c r="O1" s="1" t="s">
+      <c r="M1" s="8"/>
+      <c r="N1" s="8"/>
+      <c r="O1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="P1" s="1"/>
-      <c r="Q1" s="1"/>
-      <c r="R1" s="3" t="s">
+      <c r="P1" s="5"/>
+      <c r="Q1" s="5"/>
+      <c r="R1" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="S1" s="6"/>
+      <c r="T1" s="6"/>
+      <c r="U1" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="V1" s="5"/>
+      <c r="W1" s="5"/>
+      <c r="X1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="S1" s="3"/>
-      <c r="T1" s="3"/>
-      <c r="U1" s="9" t="s">
+      <c r="Y1" s="6"/>
+      <c r="Z1" s="6"/>
+      <c r="AA1" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="V1" s="9"/>
-      <c r="W1" s="9"/>
-      <c r="X1" s="10" t="s">
+      <c r="AB1" s="9"/>
+      <c r="AC1" s="9"/>
+      <c r="AD1" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="Y1" s="10"/>
-      <c r="Z1" s="10"/>
-      <c r="AA1" s="1" t="s">
+      <c r="AE1" s="10"/>
+      <c r="AF1" s="10"/>
+      <c r="AG1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="AB1" s="1"/>
-      <c r="AC1" s="1"/>
-      <c r="AD1" s="3" t="s">
+      <c r="AH1" s="5"/>
+      <c r="AI1" s="5"/>
+      <c r="AJ1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="AE1" s="3"/>
-      <c r="AF1" s="3"/>
+      <c r="AK1" s="6"/>
+      <c r="AL1" s="6"/>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:38" x14ac:dyDescent="0.5">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="1">
         <v>7</v>
       </c>
-      <c r="D2" s="2">
-        <v>3</v>
-      </c>
-      <c r="E2" s="2">
+      <c r="D2" s="1">
+        <v>3</v>
+      </c>
+      <c r="E2" s="1">
         <f>C2*D2</f>
         <v>21</v>
       </c>
-      <c r="F2" s="4">
+      <c r="F2" s="2">
         <v>9</v>
       </c>
-      <c r="G2" s="4">
-        <v>2</v>
-      </c>
-      <c r="H2" s="4">
+      <c r="G2" s="2">
+        <v>2</v>
+      </c>
+      <c r="H2" s="2">
         <f>F2*G2</f>
         <v>18</v>
       </c>
-      <c r="I2" s="6">
+      <c r="I2" s="3">
         <v>6</v>
       </c>
-      <c r="J2" s="6">
-        <v>3</v>
-      </c>
-      <c r="K2" s="6">
+      <c r="J2" s="3">
+        <v>3</v>
+      </c>
+      <c r="K2" s="3">
         <f>I2*J2</f>
         <v>18</v>
       </c>
-      <c r="L2" s="8">
+      <c r="L2" s="4">
         <v>5</v>
       </c>
-      <c r="M2" s="8">
-        <v>4</v>
-      </c>
-      <c r="N2" s="8">
+      <c r="M2" s="4">
+        <v>4</v>
+      </c>
+      <c r="N2" s="4">
         <f>L2*M2</f>
         <v>20</v>
       </c>
-      <c r="O2" s="2">
+      <c r="O2" s="1">
         <v>10</v>
       </c>
-      <c r="P2" s="2">
-        <v>2</v>
-      </c>
-      <c r="Q2" s="2">
+      <c r="P2" s="1">
+        <v>2</v>
+      </c>
+      <c r="Q2" s="1">
         <f>O2*P2</f>
         <v>20</v>
       </c>
-      <c r="R2" s="4">
-        <v>3</v>
-      </c>
-      <c r="S2" s="4">
-        <v>2</v>
-      </c>
-      <c r="T2" s="4">
+      <c r="R2" s="2">
+        <v>6</v>
+      </c>
+      <c r="S2" s="2">
+        <v>4</v>
+      </c>
+      <c r="T2" s="2">
         <f>R2*S2</f>
+        <v>24</v>
+      </c>
+      <c r="U2" s="1">
         <v>6</v>
       </c>
-      <c r="U2" s="6">
+      <c r="V2" s="1">
+        <v>4</v>
+      </c>
+      <c r="W2" s="1">
+        <f>U2*V2</f>
+        <v>24</v>
+      </c>
+      <c r="X2" s="2">
+        <v>3</v>
+      </c>
+      <c r="Y2" s="2">
+        <v>2</v>
+      </c>
+      <c r="Z2" s="2">
+        <f>X2*Y2</f>
+        <v>6</v>
+      </c>
+      <c r="AA2" s="3">
         <v>5</v>
       </c>
-      <c r="V2" s="6">
-        <v>4</v>
-      </c>
-      <c r="W2" s="6">
-        <f>U2*V2</f>
+      <c r="AB2" s="3">
+        <v>4</v>
+      </c>
+      <c r="AC2" s="3">
+        <f>AA2*AB2</f>
         <v>20</v>
       </c>
-      <c r="X2" s="8">
+      <c r="AD2" s="4">
         <v>9</v>
-      </c>
-      <c r="Y2" s="8">
-        <v>2</v>
-      </c>
-      <c r="Z2" s="8">
-        <f>X2*Y2</f>
-        <v>18</v>
-      </c>
-      <c r="AA2" s="2">
-        <v>7</v>
-      </c>
-      <c r="AB2" s="2">
-        <v>3</v>
-      </c>
-      <c r="AC2" s="2">
-        <f>AA2*AB2</f>
-        <v>21</v>
-      </c>
-      <c r="AD2" s="4">
-        <v>8</v>
       </c>
       <c r="AE2" s="4">
         <v>2</v>
       </c>
       <c r="AF2" s="4">
         <f>AD2*AE2</f>
+        <v>18</v>
+      </c>
+      <c r="AG2" s="1">
+        <v>7</v>
+      </c>
+      <c r="AH2" s="1">
+        <v>3</v>
+      </c>
+      <c r="AI2" s="1">
+        <f>AG2*AH2</f>
+        <v>21</v>
+      </c>
+      <c r="AJ2" s="2">
+        <v>8</v>
+      </c>
+      <c r="AK2" s="2">
+        <v>2</v>
+      </c>
+      <c r="AL2" s="2">
+        <f>AJ2*AK2</f>
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:38" x14ac:dyDescent="0.5">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="1">
         <v>9</v>
       </c>
-      <c r="D3" s="2">
-        <v>3</v>
-      </c>
-      <c r="E3" s="2">
+      <c r="D3" s="1">
+        <v>3</v>
+      </c>
+      <c r="E3" s="1">
         <f t="shared" ref="E3:E8" si="0">C3*D3</f>
         <v>27</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F3" s="2">
         <v>12</v>
       </c>
-      <c r="G3" s="4">
-        <v>2</v>
-      </c>
-      <c r="H3" s="4">
+      <c r="G3" s="2">
+        <v>2</v>
+      </c>
+      <c r="H3" s="2">
         <f t="shared" ref="H3:H8" si="1">F3*G3</f>
         <v>24</v>
       </c>
-      <c r="I3" s="6">
+      <c r="I3" s="3">
         <v>7</v>
       </c>
-      <c r="J3" s="6">
-        <v>3</v>
-      </c>
-      <c r="K3" s="6">
+      <c r="J3" s="3">
+        <v>3</v>
+      </c>
+      <c r="K3" s="3">
         <f t="shared" ref="K3:K8" si="2">I3*J3</f>
         <v>21</v>
       </c>
-      <c r="L3" s="8">
+      <c r="L3" s="4">
         <v>6</v>
       </c>
-      <c r="M3" s="8">
-        <v>4</v>
-      </c>
-      <c r="N3" s="8">
+      <c r="M3" s="4">
+        <v>4</v>
+      </c>
+      <c r="N3" s="4">
         <f t="shared" ref="N3:N8" si="3">L3*M3</f>
         <v>24</v>
       </c>
-      <c r="O3" s="2">
+      <c r="O3" s="1">
         <v>13</v>
       </c>
-      <c r="P3" s="2">
-        <v>2</v>
-      </c>
-      <c r="Q3" s="2">
+      <c r="P3" s="1">
+        <v>2</v>
+      </c>
+      <c r="Q3" s="1">
         <f t="shared" ref="Q3:Q8" si="4">O3*P3</f>
         <v>26</v>
       </c>
-      <c r="R3" s="4">
-        <v>5</v>
-      </c>
-      <c r="S3" s="4">
-        <v>2</v>
-      </c>
-      <c r="T3" s="4">
+      <c r="R3" s="2">
+        <v>7</v>
+      </c>
+      <c r="S3" s="2">
+        <v>4</v>
+      </c>
+      <c r="T3" s="2">
         <f t="shared" ref="T3:T8" si="5">R3*S3</f>
-        <v>10</v>
-      </c>
-      <c r="U3" s="6">
+        <v>28</v>
+      </c>
+      <c r="U3" s="1">
         <v>7</v>
       </c>
-      <c r="V3" s="6">
-        <v>4</v>
-      </c>
-      <c r="W3" s="6">
+      <c r="V3" s="1">
+        <v>4</v>
+      </c>
+      <c r="W3" s="1">
         <f t="shared" ref="W3:W8" si="6">U3*V3</f>
         <v>28</v>
       </c>
-      <c r="X3" s="8">
+      <c r="X3" s="2">
+        <v>5</v>
+      </c>
+      <c r="Y3" s="2">
+        <v>2</v>
+      </c>
+      <c r="Z3" s="2">
+        <f t="shared" ref="Z3:Z8" si="7">X3*Y3</f>
+        <v>10</v>
+      </c>
+      <c r="AA3" s="3">
+        <v>7</v>
+      </c>
+      <c r="AB3" s="3">
+        <v>4</v>
+      </c>
+      <c r="AC3" s="3">
+        <f t="shared" ref="AC3:AC8" si="8">AA3*AB3</f>
+        <v>28</v>
+      </c>
+      <c r="AD3" s="4">
         <v>11</v>
-      </c>
-      <c r="Y3" s="8">
-        <v>2</v>
-      </c>
-      <c r="Z3" s="8">
-        <f t="shared" ref="Z3:Z8" si="7">X3*Y3</f>
-        <v>22</v>
-      </c>
-      <c r="AA3" s="2">
-        <v>9</v>
-      </c>
-      <c r="AB3" s="2">
-        <v>3</v>
-      </c>
-      <c r="AC3" s="2">
-        <f t="shared" ref="AC3:AC8" si="8">AA3*AB3</f>
-        <v>27</v>
-      </c>
-      <c r="AD3" s="4">
-        <v>10</v>
       </c>
       <c r="AE3" s="4">
         <v>2</v>
       </c>
       <c r="AF3" s="4">
         <f t="shared" ref="AF3:AF8" si="9">AD3*AE3</f>
+        <v>22</v>
+      </c>
+      <c r="AG3" s="1">
+        <v>9</v>
+      </c>
+      <c r="AH3" s="1">
+        <v>3</v>
+      </c>
+      <c r="AI3" s="1">
+        <f t="shared" ref="AI3:AI8" si="10">AG3*AH3</f>
+        <v>27</v>
+      </c>
+      <c r="AJ3" s="2">
+        <v>10</v>
+      </c>
+      <c r="AK3" s="2">
+        <v>2</v>
+      </c>
+      <c r="AL3" s="2">
+        <f t="shared" ref="AL3:AL8" si="11">AJ3*AK3</f>
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:38" x14ac:dyDescent="0.5">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4">
         <v>2</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="1">
         <v>11</v>
       </c>
-      <c r="D4" s="2">
-        <v>3</v>
-      </c>
-      <c r="E4" s="2">
-        <f t="shared" ref="E4" si="10">C4*D4</f>
+      <c r="D4" s="1">
+        <v>3</v>
+      </c>
+      <c r="E4" s="1">
+        <f t="shared" ref="E4" si="12">C4*D4</f>
         <v>33</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4" s="2">
         <v>15</v>
       </c>
-      <c r="G4" s="4">
-        <v>2</v>
-      </c>
-      <c r="H4" s="4">
-        <f t="shared" ref="H4" si="11">F4*G4</f>
+      <c r="G4" s="2">
+        <v>2</v>
+      </c>
+      <c r="H4" s="2">
+        <f t="shared" ref="H4" si="13">F4*G4</f>
         <v>30</v>
       </c>
-      <c r="I4" s="6">
+      <c r="I4" s="3">
         <v>8</v>
       </c>
-      <c r="J4" s="6">
-        <v>3</v>
-      </c>
-      <c r="K4" s="6">
-        <f t="shared" ref="K4" si="12">I4*J4</f>
+      <c r="J4" s="3">
+        <v>3</v>
+      </c>
+      <c r="K4" s="3">
+        <f t="shared" ref="K4" si="14">I4*J4</f>
         <v>24</v>
       </c>
-      <c r="L4" s="8">
+      <c r="L4" s="4">
         <v>7</v>
       </c>
-      <c r="M4" s="8">
-        <v>4</v>
-      </c>
-      <c r="N4" s="8">
-        <f t="shared" ref="N4" si="13">L4*M4</f>
+      <c r="M4" s="4">
+        <v>4</v>
+      </c>
+      <c r="N4" s="4">
+        <f t="shared" ref="N4" si="15">L4*M4</f>
         <v>28</v>
       </c>
-      <c r="O4" s="2">
+      <c r="O4" s="1">
         <v>16</v>
       </c>
-      <c r="P4" s="2">
-        <v>2</v>
-      </c>
-      <c r="Q4" s="2">
-        <f t="shared" ref="Q4" si="14">O4*P4</f>
+      <c r="P4" s="1">
+        <v>2</v>
+      </c>
+      <c r="Q4" s="1">
+        <f t="shared" ref="Q4" si="16">O4*P4</f>
         <v>32</v>
       </c>
-      <c r="R4" s="4">
+      <c r="R4" s="2">
+        <v>9</v>
+      </c>
+      <c r="S4" s="2">
+        <v>4</v>
+      </c>
+      <c r="T4" s="2">
+        <f t="shared" si="5"/>
+        <v>36</v>
+      </c>
+      <c r="U4" s="1">
+        <v>9</v>
+      </c>
+      <c r="V4" s="1">
+        <v>4</v>
+      </c>
+      <c r="W4" s="1">
+        <f t="shared" si="6"/>
+        <v>36</v>
+      </c>
+      <c r="X4" s="2">
         <v>7</v>
       </c>
-      <c r="S4" s="4">
-        <v>2</v>
-      </c>
-      <c r="T4" s="4">
-        <f t="shared" ref="T4" si="15">R4*S4</f>
+      <c r="Y4" s="2">
+        <v>2</v>
+      </c>
+      <c r="Z4" s="2">
+        <f t="shared" ref="Z4" si="17">X4*Y4</f>
         <v>14</v>
       </c>
-      <c r="U4" s="6">
+      <c r="AA4" s="3">
         <v>9</v>
       </c>
-      <c r="V4" s="6">
-        <v>4</v>
-      </c>
-      <c r="W4" s="6">
-        <f t="shared" ref="W4" si="16">U4*V4</f>
+      <c r="AB4" s="3">
+        <v>4</v>
+      </c>
+      <c r="AC4" s="3">
+        <f t="shared" ref="AC4" si="18">AA4*AB4</f>
         <v>36</v>
       </c>
-      <c r="X4" s="8">
+      <c r="AD4" s="4">
         <v>13</v>
-      </c>
-      <c r="Y4" s="8">
-        <v>2</v>
-      </c>
-      <c r="Z4" s="8">
-        <f t="shared" ref="Z4" si="17">X4*Y4</f>
-        <v>26</v>
-      </c>
-      <c r="AA4" s="2">
-        <v>11</v>
-      </c>
-      <c r="AB4" s="2">
-        <v>3</v>
-      </c>
-      <c r="AC4" s="2">
-        <f t="shared" ref="AC4" si="18">AA4*AB4</f>
-        <v>33</v>
-      </c>
-      <c r="AD4" s="4">
-        <v>12</v>
       </c>
       <c r="AE4" s="4">
         <v>2</v>
       </c>
       <c r="AF4" s="4">
         <f t="shared" ref="AF4" si="19">AD4*AE4</f>
+        <v>26</v>
+      </c>
+      <c r="AG4" s="1">
+        <v>11</v>
+      </c>
+      <c r="AH4" s="1">
+        <v>3</v>
+      </c>
+      <c r="AI4" s="1">
+        <f t="shared" ref="AI4" si="20">AG4*AH4</f>
+        <v>33</v>
+      </c>
+      <c r="AJ4" s="2">
+        <v>12</v>
+      </c>
+      <c r="AK4" s="2">
+        <v>2</v>
+      </c>
+      <c r="AL4" s="2">
+        <f t="shared" ref="AL4" si="21">AJ4*AK4</f>
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:38" x14ac:dyDescent="0.5">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5">
         <v>2</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="1">
         <v>13</v>
       </c>
-      <c r="D5" s="2">
-        <v>3</v>
-      </c>
-      <c r="E5" s="2">
+      <c r="D5" s="1">
+        <v>3</v>
+      </c>
+      <c r="E5" s="1">
         <f t="shared" si="0"/>
         <v>39</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5" s="2">
         <v>18</v>
       </c>
-      <c r="G5" s="4">
-        <v>2</v>
-      </c>
-      <c r="H5" s="4">
+      <c r="G5" s="2">
+        <v>2</v>
+      </c>
+      <c r="H5" s="2">
         <f t="shared" si="1"/>
         <v>36</v>
       </c>
-      <c r="I5" s="6">
+      <c r="I5" s="3">
         <v>9</v>
       </c>
-      <c r="J5" s="6">
-        <v>3</v>
-      </c>
-      <c r="K5" s="6">
+      <c r="J5" s="3">
+        <v>3</v>
+      </c>
+      <c r="K5" s="3">
         <f t="shared" si="2"/>
         <v>27</v>
       </c>
-      <c r="L5" s="8">
+      <c r="L5" s="4">
         <v>8</v>
       </c>
-      <c r="M5" s="8">
-        <v>4</v>
-      </c>
-      <c r="N5" s="8">
+      <c r="M5" s="4">
+        <v>4</v>
+      </c>
+      <c r="N5" s="4">
         <f t="shared" si="3"/>
         <v>32</v>
       </c>
-      <c r="O5" s="2">
+      <c r="O5" s="1">
         <v>19</v>
       </c>
-      <c r="P5" s="2">
-        <v>2</v>
-      </c>
-      <c r="Q5" s="2">
+      <c r="P5" s="1">
+        <v>2</v>
+      </c>
+      <c r="Q5" s="1">
         <f t="shared" si="4"/>
         <v>38</v>
       </c>
-      <c r="R5" s="4">
+      <c r="R5" s="2">
+        <v>10</v>
+      </c>
+      <c r="S5" s="2">
+        <v>4</v>
+      </c>
+      <c r="T5" s="2">
+        <f t="shared" si="5"/>
+        <v>40</v>
+      </c>
+      <c r="U5" s="1">
+        <v>10</v>
+      </c>
+      <c r="V5" s="1">
+        <v>4</v>
+      </c>
+      <c r="W5" s="1">
+        <f t="shared" si="6"/>
+        <v>40</v>
+      </c>
+      <c r="X5" s="2">
         <v>9</v>
       </c>
-      <c r="S5" s="4">
-        <v>2</v>
-      </c>
-      <c r="T5" s="4">
-        <f t="shared" si="5"/>
+      <c r="Y5" s="2">
+        <v>2</v>
+      </c>
+      <c r="Z5" s="2">
+        <f t="shared" si="7"/>
         <v>18</v>
       </c>
-      <c r="U5" s="6">
+      <c r="AA5" s="3">
         <v>11</v>
       </c>
-      <c r="V5" s="6">
-        <v>4</v>
-      </c>
-      <c r="W5" s="6">
-        <f t="shared" si="6"/>
+      <c r="AB5" s="3">
+        <v>4</v>
+      </c>
+      <c r="AC5" s="3">
+        <f t="shared" si="8"/>
         <v>44</v>
       </c>
-      <c r="X5" s="8">
+      <c r="AD5" s="4">
         <v>15</v>
-      </c>
-      <c r="Y5" s="8">
-        <v>2</v>
-      </c>
-      <c r="Z5" s="8">
-        <f t="shared" si="7"/>
-        <v>30</v>
-      </c>
-      <c r="AA5" s="2">
-        <v>13</v>
-      </c>
-      <c r="AB5" s="2">
-        <v>3</v>
-      </c>
-      <c r="AC5" s="2">
-        <f t="shared" si="8"/>
-        <v>39</v>
-      </c>
-      <c r="AD5" s="4">
-        <v>14</v>
       </c>
       <c r="AE5" s="4">
         <v>2</v>
       </c>
       <c r="AF5" s="4">
         <f t="shared" si="9"/>
+        <v>30</v>
+      </c>
+      <c r="AG5" s="1">
+        <v>13</v>
+      </c>
+      <c r="AH5" s="1">
+        <v>3</v>
+      </c>
+      <c r="AI5" s="1">
+        <f t="shared" si="10"/>
+        <v>39</v>
+      </c>
+      <c r="AJ5" s="2">
+        <v>14</v>
+      </c>
+      <c r="AK5" s="2">
+        <v>2</v>
+      </c>
+      <c r="AL5" s="2">
+        <f t="shared" si="11"/>
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:38" x14ac:dyDescent="0.5">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6">
         <v>3</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="1">
         <v>15</v>
       </c>
-      <c r="D6" s="2">
-        <v>3</v>
-      </c>
-      <c r="E6" s="2">
-        <f t="shared" ref="E6" si="20">C6*D6</f>
+      <c r="D6" s="1">
+        <v>3</v>
+      </c>
+      <c r="E6" s="1">
+        <f t="shared" ref="E6" si="22">C6*D6</f>
         <v>45</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F6" s="2">
         <v>20</v>
       </c>
-      <c r="G6" s="4">
-        <v>2</v>
-      </c>
-      <c r="H6" s="4">
-        <f t="shared" ref="H6" si="21">F6*G6</f>
+      <c r="G6" s="2">
+        <v>2</v>
+      </c>
+      <c r="H6" s="2">
+        <f t="shared" ref="H6" si="23">F6*G6</f>
         <v>40</v>
       </c>
-      <c r="I6" s="6">
+      <c r="I6" s="3">
         <v>10</v>
       </c>
-      <c r="J6" s="6">
-        <v>3</v>
-      </c>
-      <c r="K6" s="6">
-        <f t="shared" ref="K6" si="22">I6*J6</f>
+      <c r="J6" s="3">
+        <v>3</v>
+      </c>
+      <c r="K6" s="3">
+        <f t="shared" ref="K6" si="24">I6*J6</f>
         <v>30</v>
       </c>
-      <c r="L6" s="8">
+      <c r="L6" s="4">
         <v>9</v>
       </c>
-      <c r="M6" s="8">
-        <v>4</v>
-      </c>
-      <c r="N6" s="8">
-        <f t="shared" ref="N6" si="23">L6*M6</f>
+      <c r="M6" s="4">
+        <v>4</v>
+      </c>
+      <c r="N6" s="4">
+        <f t="shared" ref="N6" si="25">L6*M6</f>
         <v>36</v>
       </c>
-      <c r="O6" s="2">
+      <c r="O6" s="1">
         <v>21</v>
       </c>
-      <c r="P6" s="2">
-        <v>2</v>
-      </c>
-      <c r="Q6" s="2">
-        <f t="shared" ref="Q6" si="24">O6*P6</f>
+      <c r="P6" s="1">
+        <v>2</v>
+      </c>
+      <c r="Q6" s="1">
+        <f t="shared" ref="Q6" si="26">O6*P6</f>
         <v>42</v>
       </c>
-      <c r="R6" s="4">
+      <c r="R6" s="2">
+        <v>12</v>
+      </c>
+      <c r="S6" s="2">
+        <v>4</v>
+      </c>
+      <c r="T6" s="2">
+        <f t="shared" si="5"/>
+        <v>48</v>
+      </c>
+      <c r="U6" s="1">
+        <v>12</v>
+      </c>
+      <c r="V6" s="1">
+        <v>4</v>
+      </c>
+      <c r="W6" s="1">
+        <f t="shared" si="6"/>
+        <v>48</v>
+      </c>
+      <c r="X6" s="2">
         <v>10</v>
       </c>
-      <c r="S6" s="4">
-        <v>2</v>
-      </c>
-      <c r="T6" s="4">
-        <f t="shared" ref="T6" si="25">R6*S6</f>
+      <c r="Y6" s="2">
+        <v>2</v>
+      </c>
+      <c r="Z6" s="2">
+        <f t="shared" ref="Z6" si="27">X6*Y6</f>
         <v>20</v>
       </c>
-      <c r="U6" s="6">
+      <c r="AA6" s="3">
         <v>12</v>
       </c>
-      <c r="V6" s="6">
-        <v>4</v>
-      </c>
-      <c r="W6" s="6">
-        <f t="shared" ref="W6" si="26">U6*V6</f>
+      <c r="AB6" s="3">
+        <v>4</v>
+      </c>
+      <c r="AC6" s="3">
+        <f t="shared" ref="AC6" si="28">AA6*AB6</f>
         <v>48</v>
       </c>
-      <c r="X6" s="8">
+      <c r="AD6" s="4">
         <v>17</v>
-      </c>
-      <c r="Y6" s="8">
-        <v>2</v>
-      </c>
-      <c r="Z6" s="8">
-        <f t="shared" ref="Z6" si="27">X6*Y6</f>
-        <v>34</v>
-      </c>
-      <c r="AA6" s="2">
-        <v>15</v>
-      </c>
-      <c r="AB6" s="2">
-        <v>3</v>
-      </c>
-      <c r="AC6" s="2">
-        <f t="shared" ref="AC6" si="28">AA6*AB6</f>
-        <v>45</v>
-      </c>
-      <c r="AD6" s="4">
-        <v>16</v>
       </c>
       <c r="AE6" s="4">
         <v>2</v>
       </c>
       <c r="AF6" s="4">
         <f t="shared" ref="AF6" si="29">AD6*AE6</f>
+        <v>34</v>
+      </c>
+      <c r="AG6" s="1">
+        <v>15</v>
+      </c>
+      <c r="AH6" s="1">
+        <v>3</v>
+      </c>
+      <c r="AI6" s="1">
+        <f t="shared" ref="AI6" si="30">AG6*AH6</f>
+        <v>45</v>
+      </c>
+      <c r="AJ6" s="2">
+        <v>16</v>
+      </c>
+      <c r="AK6" s="2">
+        <v>2</v>
+      </c>
+      <c r="AL6" s="2">
+        <f t="shared" ref="AL6" si="31">AJ6*AK6</f>
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:38" x14ac:dyDescent="0.5">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7">
         <v>3</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="1">
         <v>16</v>
       </c>
-      <c r="D7" s="2">
-        <v>3</v>
-      </c>
-      <c r="E7" s="2">
+      <c r="D7" s="1">
+        <v>3</v>
+      </c>
+      <c r="E7" s="1">
         <f t="shared" si="0"/>
         <v>48</v>
       </c>
-      <c r="F7" s="4">
+      <c r="F7" s="2">
         <v>22</v>
       </c>
-      <c r="G7" s="4">
-        <v>2</v>
-      </c>
-      <c r="H7" s="4">
+      <c r="G7" s="2">
+        <v>2</v>
+      </c>
+      <c r="H7" s="2">
         <f t="shared" si="1"/>
         <v>44</v>
       </c>
-      <c r="I7" s="6">
+      <c r="I7" s="3">
         <v>11</v>
       </c>
-      <c r="J7" s="6">
-        <v>3</v>
-      </c>
-      <c r="K7" s="6">
+      <c r="J7" s="3">
+        <v>3</v>
+      </c>
+      <c r="K7" s="3">
         <f t="shared" si="2"/>
         <v>33</v>
       </c>
-      <c r="L7" s="8">
+      <c r="L7" s="4">
         <v>10</v>
       </c>
-      <c r="M7" s="8">
-        <v>4</v>
-      </c>
-      <c r="N7" s="8">
+      <c r="M7" s="4">
+        <v>4</v>
+      </c>
+      <c r="N7" s="4">
         <f t="shared" si="3"/>
         <v>40</v>
       </c>
-      <c r="O7" s="2">
+      <c r="O7" s="1">
         <v>23</v>
       </c>
-      <c r="P7" s="2">
-        <v>2</v>
-      </c>
-      <c r="Q7" s="2">
+      <c r="P7" s="1">
+        <v>2</v>
+      </c>
+      <c r="Q7" s="1">
         <f t="shared" si="4"/>
         <v>46</v>
       </c>
-      <c r="R7" s="4">
-        <v>11</v>
-      </c>
-      <c r="S7" s="4">
-        <v>2</v>
-      </c>
-      <c r="T7" s="4">
+      <c r="R7" s="2">
+        <v>13</v>
+      </c>
+      <c r="S7" s="2">
+        <v>4</v>
+      </c>
+      <c r="T7" s="2">
         <f t="shared" si="5"/>
-        <v>22</v>
-      </c>
-      <c r="U7" s="6">
+        <v>52</v>
+      </c>
+      <c r="U7" s="1">
         <v>13</v>
       </c>
-      <c r="V7" s="6">
-        <v>4</v>
-      </c>
-      <c r="W7" s="6">
+      <c r="V7" s="1">
+        <v>4</v>
+      </c>
+      <c r="W7" s="1">
         <f t="shared" si="6"/>
         <v>52</v>
       </c>
-      <c r="X7" s="8">
+      <c r="X7" s="2">
+        <v>11</v>
+      </c>
+      <c r="Y7" s="2">
+        <v>2</v>
+      </c>
+      <c r="Z7" s="2">
+        <f t="shared" si="7"/>
+        <v>22</v>
+      </c>
+      <c r="AA7" s="3">
+        <v>13</v>
+      </c>
+      <c r="AB7" s="3">
+        <v>4</v>
+      </c>
+      <c r="AC7" s="3">
+        <f t="shared" si="8"/>
+        <v>52</v>
+      </c>
+      <c r="AD7" s="4">
         <v>19</v>
-      </c>
-      <c r="Y7" s="8">
-        <v>2</v>
-      </c>
-      <c r="Z7" s="8">
-        <f t="shared" si="7"/>
-        <v>38</v>
-      </c>
-      <c r="AA7" s="2">
-        <v>16</v>
-      </c>
-      <c r="AB7" s="2">
-        <v>3</v>
-      </c>
-      <c r="AC7" s="2">
-        <f t="shared" si="8"/>
-        <v>48</v>
-      </c>
-      <c r="AD7" s="4">
-        <v>18</v>
       </c>
       <c r="AE7" s="4">
         <v>2</v>
       </c>
       <c r="AF7" s="4">
         <f t="shared" si="9"/>
+        <v>38</v>
+      </c>
+      <c r="AG7" s="1">
+        <v>16</v>
+      </c>
+      <c r="AH7" s="1">
+        <v>3</v>
+      </c>
+      <c r="AI7" s="1">
+        <f t="shared" si="10"/>
+        <v>48</v>
+      </c>
+      <c r="AJ7" s="2">
+        <v>18</v>
+      </c>
+      <c r="AK7" s="2">
+        <v>2</v>
+      </c>
+      <c r="AL7" s="2">
+        <f t="shared" si="11"/>
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:38" x14ac:dyDescent="0.5">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8">
         <v>4</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="1">
         <v>17</v>
       </c>
-      <c r="D8" s="2">
-        <v>3</v>
-      </c>
-      <c r="E8" s="2">
+      <c r="D8" s="1">
+        <v>3</v>
+      </c>
+      <c r="E8" s="1">
         <f t="shared" si="0"/>
         <v>51</v>
       </c>
-      <c r="F8" s="4">
+      <c r="F8" s="2">
         <v>24</v>
       </c>
-      <c r="G8" s="4">
-        <v>2</v>
-      </c>
-      <c r="H8" s="4">
+      <c r="G8" s="2">
+        <v>2</v>
+      </c>
+      <c r="H8" s="2">
         <f t="shared" si="1"/>
         <v>48</v>
       </c>
-      <c r="I8" s="6">
+      <c r="I8" s="3">
         <v>12</v>
       </c>
-      <c r="J8" s="6">
-        <v>3</v>
-      </c>
-      <c r="K8" s="6">
+      <c r="J8" s="3">
+        <v>3</v>
+      </c>
+      <c r="K8" s="3">
         <f t="shared" si="2"/>
         <v>36</v>
       </c>
-      <c r="L8" s="8">
+      <c r="L8" s="4">
         <v>11</v>
       </c>
-      <c r="M8" s="8">
-        <v>4</v>
-      </c>
-      <c r="N8" s="8">
+      <c r="M8" s="4">
+        <v>4</v>
+      </c>
+      <c r="N8" s="4">
         <f t="shared" si="3"/>
         <v>44</v>
       </c>
-      <c r="O8" s="2">
+      <c r="O8" s="1">
         <v>25</v>
       </c>
-      <c r="P8" s="2">
-        <v>2</v>
-      </c>
-      <c r="Q8" s="2">
+      <c r="P8" s="1">
+        <v>2</v>
+      </c>
+      <c r="Q8" s="1">
         <f t="shared" si="4"/>
         <v>50</v>
       </c>
-      <c r="R8" s="4">
-        <v>12</v>
-      </c>
-      <c r="S8" s="4">
-        <v>2</v>
-      </c>
-      <c r="T8" s="4">
+      <c r="R8" s="2">
+        <v>14</v>
+      </c>
+      <c r="S8" s="2">
+        <v>4</v>
+      </c>
+      <c r="T8" s="2">
         <f t="shared" si="5"/>
-        <v>24</v>
-      </c>
-      <c r="U8" s="6">
+        <v>56</v>
+      </c>
+      <c r="U8" s="1">
         <v>14</v>
       </c>
-      <c r="V8" s="6">
-        <v>4</v>
-      </c>
-      <c r="W8" s="6">
+      <c r="V8" s="1">
+        <v>4</v>
+      </c>
+      <c r="W8" s="1">
         <f t="shared" si="6"/>
         <v>56</v>
       </c>
-      <c r="X8" s="8">
+      <c r="X8" s="2">
+        <v>12</v>
+      </c>
+      <c r="Y8" s="2">
+        <v>2</v>
+      </c>
+      <c r="Z8" s="2">
+        <f t="shared" si="7"/>
+        <v>24</v>
+      </c>
+      <c r="AA8" s="3">
+        <v>14</v>
+      </c>
+      <c r="AB8" s="3">
+        <v>4</v>
+      </c>
+      <c r="AC8" s="3">
+        <f t="shared" si="8"/>
+        <v>56</v>
+      </c>
+      <c r="AD8" s="4">
         <v>21</v>
-      </c>
-      <c r="Y8" s="8">
-        <v>2</v>
-      </c>
-      <c r="Z8" s="8">
-        <f t="shared" si="7"/>
-        <v>42</v>
-      </c>
-      <c r="AA8" s="2">
-        <v>17</v>
-      </c>
-      <c r="AB8" s="2">
-        <v>3</v>
-      </c>
-      <c r="AC8" s="2">
-        <f t="shared" si="8"/>
-        <v>51</v>
-      </c>
-      <c r="AD8" s="4">
-        <v>20</v>
       </c>
       <c r="AE8" s="4">
         <v>2</v>
       </c>
       <c r="AF8" s="4">
         <f t="shared" si="9"/>
+        <v>42</v>
+      </c>
+      <c r="AG8" s="1">
+        <v>17</v>
+      </c>
+      <c r="AH8" s="1">
+        <v>3</v>
+      </c>
+      <c r="AI8" s="1">
+        <f t="shared" si="10"/>
+        <v>51</v>
+      </c>
+      <c r="AJ8" s="2">
+        <v>20</v>
+      </c>
+      <c r="AK8" s="2">
+        <v>2</v>
+      </c>
+      <c r="AL8" s="2">
+        <f t="shared" si="11"/>
         <v>40</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="U1:W1"/>
-    <mergeCell ref="X1:Z1"/>
+  <mergeCells count="12">
     <mergeCell ref="AA1:AC1"/>
     <mergeCell ref="AD1:AF1"/>
+    <mergeCell ref="AG1:AI1"/>
+    <mergeCell ref="AJ1:AL1"/>
     <mergeCell ref="C1:E1"/>
     <mergeCell ref="F1:H1"/>
     <mergeCell ref="I1:K1"/>
     <mergeCell ref="L1:N1"/>
     <mergeCell ref="O1:Q1"/>
+    <mergeCell ref="X1:Z1"/>
     <mergeCell ref="R1:T1"/>
+    <mergeCell ref="U1:W1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>